<commit_message>
Added entry into activity log
</commit_message>
<xml_diff>
--- a/jaclemon.xlsx
+++ b/jaclemon.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorda\OneDrive\Desktop\306\PRE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorda\306PRE_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1B597F-700B-4CD4-B3ED-82E1E292DFA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12302E0C-95A6-47B9-8DF0-D30982A476A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>DATE</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>ACTIVITY &amp; TOOL DESCRIPTION</t>
+  </si>
+  <si>
+    <t>jaclemon</t>
+  </si>
+  <si>
+    <t>60 minutes</t>
+  </si>
+  <si>
+    <t>Setting up Github repo for project</t>
   </si>
 </sst>
 </file>
@@ -72,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -380,6 +390,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43864</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added command line aruement reader
</commit_message>
<xml_diff>
--- a/jaclemon.xlsx
+++ b/jaclemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorda\306PRE_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12302E0C-95A6-47B9-8DF0-D30982A476A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F493A3AE-64AB-4D8F-9C8A-C544D355AE80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>DATE</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>Setting up Github repo for project</t>
+  </si>
+  <si>
+    <t>Wrote function to read command line arguments using notepad++</t>
+  </si>
+  <si>
+    <t>30 minutes</t>
+  </si>
+  <si>
+    <t>Used notepad++ to fix exit status and deleted branch and added all changes to master with github</t>
   </si>
 </sst>
 </file>
@@ -364,16 +373,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="4" max="4" width="55.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -404,6 +413,34 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43865</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43866</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented min and mean functions/updated activity log
</commit_message>
<xml_diff>
--- a/jaclemon.xlsx
+++ b/jaclemon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorda\306PRE_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F493A3AE-64AB-4D8F-9C8A-C544D355AE80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206FE874-8320-4970-AA64-DCBB3A4D42AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>DATE</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>Used notepad++ to fix exit status and deleted branch and added all changes to master with github</t>
+  </si>
+  <si>
+    <t>Used notepad++ to try and diagnose segmentation fault error with csvreader</t>
+  </si>
+  <si>
+    <t>2/13/2020jaclemon</t>
+  </si>
+  <si>
+    <t>Used notepad++ to implement -min, -mean functions</t>
   </si>
 </sst>
 </file>
@@ -373,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,6 +450,31 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43870</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed -r read issue/updated activity log
</commit_message>
<xml_diff>
--- a/jaclemon.xlsx
+++ b/jaclemon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorda\306PRE_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206FE874-8320-4970-AA64-DCBB3A4D42AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356BD7B1-CD6F-4EBA-B0A9-703C4D2029CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>DATE</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Used notepad++ to implement -min, -mean functions</t>
+  </si>
+  <si>
+    <t>20 minutes</t>
+  </si>
+  <si>
+    <t>Used Clion to fix command line issue where -records would read as -r</t>
   </si>
 </sst>
 </file>
@@ -382,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,6 +481,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added functionality to prevent command args being repeated from having an affect
</commit_message>
<xml_diff>
--- a/jaclemon.xlsx
+++ b/jaclemon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorda\306PRE_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356BD7B1-CD6F-4EBA-B0A9-703C4D2029CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB57F7A5-85A4-4F5E-989D-079EC5A33BB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="4155" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>DATE</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Used Clion to fix command line issue where -records would read as -r</t>
+  </si>
+  <si>
+    <t>15 minutes</t>
+  </si>
+  <si>
+    <t>Used Clion to prevent from repeated command lines from having an affect</t>
   </si>
 </sst>
 </file>
@@ -388,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,6 +498,17 @@
         <v>14</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added functionality to recognize illegal command line args/updated log
</commit_message>
<xml_diff>
--- a/jaclemon.xlsx
+++ b/jaclemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorda\306PRE_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB57F7A5-85A4-4F5E-989D-079EC5A33BB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A64A88-1936-4298-BC6D-1687A8D2FDB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4155" yWindow="4155" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>DATE</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Used Clion to prevent from repeated command lines from having an affect</t>
+  </si>
+  <si>
+    <t>Used Clion to recognize illegal command line args</t>
   </si>
 </sst>
 </file>
@@ -394,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,6 +512,17 @@
         <v>16</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed illegal command error/updated log
</commit_message>
<xml_diff>
--- a/jaclemon.xlsx
+++ b/jaclemon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorda\306PRE_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A64A88-1936-4298-BC6D-1687A8D2FDB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A056B1D1-3527-472C-82F4-E0F8A536E241}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="4155" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>DATE</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Used Clion to recognize illegal command line args</t>
+  </si>
+  <si>
+    <t>45 minutes</t>
+  </si>
+  <si>
+    <t>Used Clion to diagnose illegal command error</t>
   </si>
 </sst>
 </file>
@@ -397,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
@@ -523,6 +529,17 @@
         <v>17</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>